<commit_message>
added support for postcoordinations; changed Name in csv column to name
</commit_message>
<xml_diff>
--- a/TRICC/formheader_cht.xlsx
+++ b/TRICC/formheader_cht.xlsx
@@ -605,25 +605,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="1"/>
-    <col min="5" max="5" width="23.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="1" customWidth="1"/>
-    <col min="9" max="1009" width="8.5703125" style="1"/>
-    <col min="1010" max="1023" width="9.140625" style="2" customWidth="1"/>
-    <col min="1024" max="1024" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" style="1"/>
+    <col min="5" max="5" width="23.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.26953125" style="1" customWidth="1"/>
+    <col min="9" max="1009" width="8.54296875" style="1"/>
+    <col min="1010" max="1023" width="9.1796875" style="2" customWidth="1"/>
+    <col min="1024" max="1024" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>

<commit_message>
Fix: :sparkles: updated script to run LBY
</commit_message>
<xml_diff>
--- a/TRICC/formheader_cht.xlsx
+++ b/TRICC/formheader_cht.xlsx
@@ -161,13 +161,13 @@
     <t>ID of the case, autogenerated</t>
   </si>
   <si>
-    <t>data_load_removesuffix</t>
-  </si>
-  <si>
-    <t>../inputs/contact/data_load_removesuffix</t>
-  </si>
-  <si>
     <t>../inputs/source_id</t>
+  </si>
+  <si>
+    <t>data_load</t>
+  </si>
+  <si>
+    <t>../inputs/contact/data_load</t>
   </si>
 </sst>
 </file>
@@ -608,22 +608,22 @@
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="1"/>
-    <col min="5" max="5" width="23.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="41.26953125" style="1" customWidth="1"/>
-    <col min="9" max="1009" width="8.54296875" style="1"/>
-    <col min="1010" max="1023" width="9.1796875" style="2" customWidth="1"/>
-    <col min="1024" max="1024" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1"/>
+    <col min="5" max="5" width="23.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" style="1" customWidth="1"/>
+    <col min="9" max="1009" width="8.5703125" style="1"/>
+    <col min="1010" max="1023" width="9.140625" style="2" customWidth="1"/>
+    <col min="1024" max="1024" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -797,7 +797,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
@@ -889,7 +889,7 @@
         <v>42</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1024">
@@ -906,7 +906,7 @@
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>

</xml_diff>